<commit_message>
update on deletion and modification
Update
</commit_message>
<xml_diff>
--- a/Product_Backlog/Product-backlog-updated.xlsx
+++ b/Product_Backlog/Product-backlog-updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stormfront/Desktop/GITHUB/Sites/DCDLEAFY.github.io/Product_Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE02657-51B7-3C4A-9D4A-A18ED691FBA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4E257D-241B-5546-8FBA-86C13A4C4BBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" xr2:uid="{292A808A-4F52-0A42-9F4B-AA9622F6EB74}"/>
   </bookViews>
@@ -261,17 +261,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ACBC413-FD9E-E84C-96CC-5F3F790D98F3}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" zoomScale="116" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,7 +621,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2">
@@ -649,7 +649,7 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="2">
         <v>2</v>
       </c>
@@ -666,12 +666,12 @@
         <v>22</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="2">
         <v>3</v>
       </c>
@@ -688,12 +688,12 @@
         <v>22</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="2">
         <v>4</v>
       </c>
@@ -710,12 +710,12 @@
         <v>24</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="2">
         <v>5</v>
       </c>
@@ -733,7 +733,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="5">
@@ -753,7 +753,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="5">
         <v>7</v>
       </c>
@@ -779,7 +779,7 @@
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="5">
         <v>8</v>
       </c>
@@ -801,7 +801,7 @@
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="5">
         <v>9</v>
       </c>
@@ -823,7 +823,7 @@
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="5">
         <v>10</v>
       </c>
@@ -841,7 +841,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="5">
         <v>11</v>
       </c>
@@ -859,7 +859,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="5">
         <v>12</v>
       </c>
@@ -875,15 +875,15 @@
       <c r="F13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="5">
         <v>13</v>
       </c>
@@ -894,7 +894,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>26</v>
@@ -913,7 +913,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5">
         <v>14</v>
       </c>
@@ -943,7 +943,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="5">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Small update on product backlog
Added what we have completed so far in the sprint in the product backlog
</commit_message>
<xml_diff>
--- a/Product_Backlog/Product-backlog-updated.xlsx
+++ b/Product_Backlog/Product-backlog-updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stormfront/Desktop/GITHUB/Sites/DCDLEAFY.github.io/Product_Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4E257D-241B-5546-8FBA-86C13A4C4BBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4DD628-0FE9-2F4E-ABB0-2EA52B55F634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" xr2:uid="{292A808A-4F52-0A42-9F4B-AA9622F6EB74}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>New points for the sprint backlog founded from sprint 2 for sprint 3:</t>
+  </si>
+  <si>
+    <t>Completed || 03/02 - 04/02</t>
   </si>
 </sst>
 </file>
@@ -590,7 +593,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -749,7 +752,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -855,7 +858,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Modified docs and excel
Modified files
</commit_message>
<xml_diff>
--- a/Product_Backlog/Product-backlog-updated.xlsx
+++ b/Product_Backlog/Product-backlog-updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stormfront/Desktop/GITHUB/Sites/DCDLEAFY.github.io/Product_Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4DD628-0FE9-2F4E-ABB0-2EA52B55F634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92A6304-6D89-CA45-AE69-3B3D44BBE96F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" xr2:uid="{292A808A-4F52-0A42-9F4B-AA9622F6EB74}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -138,6 +138,48 @@
   </si>
   <si>
     <t>Completed || 03/02 - 04/02</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Completed || 03/02 - 05/02</t>
+  </si>
+  <si>
+    <t>Completed || 05/02 - 06/02</t>
+  </si>
+  <si>
+    <t>Completed || 04/02 - 06/02</t>
+  </si>
+  <si>
+    <t>Completed || 06/02 - 07/02</t>
+  </si>
+  <si>
+    <t>Completed || 04/02 - 05/02</t>
+  </si>
+  <si>
+    <t>Completed || 05/02 - 07/02</t>
+  </si>
+  <si>
+    <t>User should be able to differentiate between markers on map</t>
+  </si>
+  <si>
+    <t>User should be able to get an update on the table when distance radius is lowered</t>
+  </si>
+  <si>
+    <t>User should be able to change distance radius when map is displayed</t>
+  </si>
+  <si>
+    <t>Incompleted ||</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QoL </t>
+  </si>
+  <si>
+    <t>Userbility and making sure that the user is getting correct info</t>
+  </si>
+  <si>
+    <t>From sprint Review</t>
   </si>
 </sst>
 </file>
@@ -590,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ACBC413-FD9E-E84C-96CC-5F3F790D98F3}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -603,7 +645,7 @@
     <col min="6" max="6" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="86.33203125" customWidth="1"/>
     <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
@@ -668,8 +710,12 @@
       <c r="F3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="15"/>
+      <c r="H3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>46</v>
+      </c>
       <c r="J3" s="15"/>
       <c r="K3" s="15"/>
     </row>
@@ -690,8 +736,12 @@
       <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="15"/>
+      <c r="H4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
     </row>
@@ -712,8 +762,12 @@
       <c r="F5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="15"/>
+      <c r="H5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
     </row>
@@ -770,7 +824,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>28</v>
@@ -796,12 +850,16 @@
         <v>4</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
@@ -818,7 +876,7 @@
         <v>4</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="2"/>
@@ -840,7 +898,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -876,7 +934,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>27</v>
@@ -900,7 +958,7 @@
         <v>4</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>17</v>
@@ -930,7 +988,7 @@
         <v>3</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="H15" s="10" t="s">
         <v>18</v>
@@ -960,7 +1018,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>19</v>
@@ -975,7 +1033,25 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="8:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="4">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="H17" s="10" t="s">
         <v>20</v>
       </c>
@@ -989,8 +1065,46 @@
         <v>26</v>
       </c>
     </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="13"/>
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="4">
+        <v>9</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="13"/>
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="4">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2">
+        <v>8</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="I9:K9"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A16"/>
     <mergeCell ref="H13:K13"/>

</xml_diff>